<commit_message>
[이용섭] Fixed - [ItemData/Table] 'Item'->'ItemData' 로 테이블 이름 변경, ImagePath 칼럼 및 데이터 추가.
Add - [Item/Image] 아이템 이미지 15종 추가 및 경로 테이블 데이터 추가.

Add - [StorageStatusModal/Widget] 스토리지 관리형 모달창 내 슬롯 관리 위젯 기능 추가.
</commit_message>
<xml_diff>
--- a/Content/TableData/Storage.xlsx
+++ b/Content/TableData/Storage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lee\Documents\Unreal Projects\ProjectMS\Content\TableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C2A146-9138-4A27-90D8-E4D10F429097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE4BE02-1DA8-4778-8F2E-32E70D19306B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25845" yWindow="1725" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -176,12 +176,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -194,13 +209,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="나쁨" xfId="2" builtinId="27"/>
@@ -483,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="J2" sqref="A1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -503,7 +519,7 @@
     <col min="10" max="10" width="7.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -518,9 +534,8 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -535,11 +550,10 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -571,7 +585,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -603,7 +617,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -632,7 +646,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -661,7 +675,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -690,7 +704,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -719,7 +733,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>5</v>
       </c>
@@ -748,7 +762,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6</v>
       </c>
@@ -777,7 +791,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>7</v>
       </c>
@@ -806,7 +820,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>8</v>
       </c>
@@ -835,7 +849,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
[박청아] Fix - [Construct] Storage 테이블 BP로 변경
</commit_message>
<xml_diff>
--- a/Content/TableData/Storage.xlsx
+++ b/Content/TableData/Storage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lee\Documents\Unreal Projects\ProjectMS\Content\TableData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\capark2690\ProjectMS\Content\TableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE4BE02-1DA8-4778-8F2E-32E70D19306B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8043F712-39F6-4075-8CE9-BB3F899FFCB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>#</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -119,6 +119,10 @@
   </si>
   <si>
     <t>Id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SM_FUR_VS_AB</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -499,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="A1:J2"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -878,6 +882,35 @@
         <v>1009</v>
       </c>
     </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>8</v>
+      </c>
+      <c r="G14">
+        <v>1000</v>
+      </c>
+      <c r="H14" s="3">
+        <v>4010</v>
+      </c>
+      <c r="I14" s="3">
+        <v>1009</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[이용섭] Add - [Prop] Palette 1종 추가 Fixed - [Palette/Prop] 프롭 테이블화 및 Storage 존타입 구분화.
</commit_message>
<xml_diff>
--- a/Content/TableData/Storage.xlsx
+++ b/Content/TableData/Storage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\capark2690\ProjectMS\Content\TableData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lee\Documents\Unreal Projects\ProjectMS\Content\TableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4C43C5-4C2A-41AA-B0CC-9C79B45FC77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8695A3B-D3EA-4504-A696-A1D9852613DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21495" yWindow="4710" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>#</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -83,45 +83,42 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>SM_FUR_DIS_A</t>
-  </si>
-  <si>
-    <t>SM_FUR_FG_A</t>
-  </si>
-  <si>
-    <t>SM_FUR_FZ_A</t>
-  </si>
-  <si>
-    <t>SM_FUR_RT_A</t>
-  </si>
-  <si>
-    <t>SM_FUR_VS_B</t>
-  </si>
-  <si>
     <t>Id</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>SM_FUR_COT_A</t>
-  </si>
-  <si>
-    <t>SM_FUR_COT_B</t>
-  </si>
-  <si>
-    <t>SM_FUR_FG_B</t>
-  </si>
-  <si>
-    <t>SM_FUR_VS_A</t>
-  </si>
-  <si>
-    <t>SM_FUR_VS_AB</t>
-  </si>
-  <si>
-    <t>SM_WH_RACK</t>
-  </si>
-  <si>
     <t>ZoneType</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cashier's desk 1</t>
+  </si>
+  <si>
+    <t>cashier's desk 2</t>
+  </si>
+  <si>
+    <t>Normal Display 1</t>
+  </si>
+  <si>
+    <t>refrigeration 1</t>
+  </si>
+  <si>
+    <t>refrigeration 2</t>
+  </si>
+  <si>
+    <t>Frozen Display 1</t>
+  </si>
+  <si>
+    <t>Normal Display 2</t>
+  </si>
+  <si>
+    <t>Fresh Display 1</t>
+  </si>
+  <si>
+    <t>Palette</t>
+  </si>
+  <si>
+    <t>Shelf Stand 1</t>
   </si>
 </sst>
 </file>
@@ -504,7 +501,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="A5" sqref="A5:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -557,10 +554,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -630,7 +627,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E5" s="3">
         <v>1</v>
@@ -659,7 +656,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E6" s="3">
         <v>1</v>
@@ -688,7 +685,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
@@ -717,7 +714,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E8" s="3">
         <v>1</v>
@@ -746,7 +743,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E9" s="3">
         <v>1</v>
@@ -775,7 +772,7 @@
         <v>3</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E10" s="3">
         <v>1</v>
@@ -804,7 +801,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E11" s="3">
         <v>1</v>
@@ -862,7 +859,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
@@ -885,7 +882,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C14" s="3">
         <v>2</v>
@@ -903,10 +900,10 @@
         <v>1000</v>
       </c>
       <c r="H14" s="3">
-        <v>4010</v>
+        <v>4012</v>
       </c>
       <c r="I14" s="3">
-        <v>1009</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -914,7 +911,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>

</xml_diff>